<commit_message>
Mostrar marcaciones, logo de la empresa y arreglos en calendario, solicitudes y justificaciones
</commit_message>
<xml_diff>
--- a/vista/archivos/asistencias.xlsx
+++ b/vista/archivos/asistencias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yo mismo\Documents\Sergio\Facultad\Sistema RRHH\Asistencias_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\facultad\rrhh\vista\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +464,216 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43102</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43102</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43102</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43102</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43102</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43103</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43103</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43103</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43103</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43103</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F16" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43104</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43104</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43104</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43104</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43104</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F21" s="3">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>